<commit_message>
Bug fix: interview, wrk exp & minor error msg
</commit_message>
<xml_diff>
--- a/data/UCL/program_details_sample.xlsx
+++ b/data/UCL/program_details_sample.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,30 +559,35 @@
       </c>
       <c r="AB1" t="inlineStr">
         <is>
+          <t>工作经验细则</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
           <t>作品集</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>GMAT</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>GRE</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>该专业对本地学生要求</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>英国本地要求展示用</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>专业细分方向</t>
         </is>
@@ -674,11 +679,6 @@
           <t>未要求</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
       <c r="AC2" t="inlineStr">
         <is>
           <t>未要求</t>
@@ -691,10 +691,15 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>未找到, 项目页面不可用或者正在更新</t>
+          <t>未要求</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
+        <is>
+          <t>2:1</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>2:1</t>
         </is>
@@ -728,20 +733,280 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>audiology</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Applicants need to have at least two years' recent post-qualification clinical experience in audiology or a related discipline. A minimum of a second-class Bachelor's degree in a relevant discipline from a UK university or an overseas qualification of an equivalent standard is the standard entry requirement.The Ear Institute recognises that some audiology professionals may have had different (non-degree) entries into the profession. Applicants with the BAAT qualification and/or a Certificate or Diploma in Hearing Therapy who also have at least five years of relevant clinical experience and appropriate registration with the RCCP may be accepted, depending on their relevant experience, and are encouraged to contact the Ear Institute to discuss their application.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Advanced Audiology is designed for practising audiologists looking to enhance their clinical skills. Graduates are eligible to apply for senior clinical roles in the NHS or private sector. A variety of specialist modules can be selected to suit your professional needs. The programme has a strong research and evidence-based practice foundation.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Advanced Audiology: Research Project
+Anatomy and Physiology of the Audio-Vestibular System
+Research Methods and Statistics
+Counselling
+Balance
+Signals, Systems, Acoustics and the Ear
+Auditory Processing and Related Disorders
+Vestibular Rehabilitation
+Paediatric Habilitation
+Advances in Auditory Implants
+Advanced Management of Tinnitus and Hyperacusis
+Paediatric Assessment
+Advanced adult rehabilitation</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/advanced-audiology-msc</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1 calendar year (full-time)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>September 2023</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>£32,100</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>总分 6.5, 小分 6.0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>需要</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+entry requirements
+applicants need to have at least two years' recent post-qualification clinical experience in audiology or a related discipline. applicants with the baat qualification and/or a certificate or diploma in hearing therapy who also have at least five years of relevant clinical experience and appropriate registration with the rccp may be accepted, depending on their relevant experience, and are encouraged to contact the ear institute to discuss their application. applicants with the baat qualification and/or a certificate or diploma in hearing therapy who also have at least five years of relevant clinical experience and appropriate registration with the rccp may be accepted, depending on their relevant experience, and are encouraged to contact the ear institute to discuss their application. 
+entry requirements
+applicants need to have at least two years' recent post-qualification clinical experience in audiology or a related discipline.</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>University College London</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>伦敦大学学院</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>global management of natural resources msc</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Normally a minimum of a second-class Bachelor’s degree in a relevant discipline – preferably engineering, Earth sciences, chemistry or finance/business - from a UK university or an overseas qualification of an equivalent standard. Relevant work experience may be taken into account.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>More than ever, there is a growing demand for versatile specialists and managers in the globalised natural resources and commodities industries. These industries rely on effective collaboration between scientists, engineers, analysts, managers, and investors. This programme gives students the opportunity to develop an integrated understanding of resource genesis, production, supply, socio-environmental footprint and sustainable practice, which is now essential.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Natural Gas Processing
+Minerals Usage, Extraction and Processing
+Prevention and Remediation of Environmental Contamination
+Dissertation
+Social Licensing
+Earth Resources and Sustainability
+Decision and Risk Analysis
+Business and Sustainability
+Renewable Energy in the Resources Sector
+Integrated Hydrogeology and Sustainable Water Management
+Geology for Global Managers and Engineers</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/global-management-natural-resources-msc</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1 calendar year (full-time)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>September 2023</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>£38,300</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>总分 6.5, 小分 6.0</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>relevant work experience may be taken into account. relevant work experience may be taken into account.</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>2:2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>英国</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>University College London</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>伦敦大学学院</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>civil engineering (with fluids) msc</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>A minimum of an upper second-class UK Bachelor's degree in civil or structural engineering or a closely related subject, or an overseas qualification of an equivalent standard. Applicants with a good performance in the core subjects (design, structures, geotechnics, and fluids) or extensive work experience covering these areas may be considered. For non-civil or structural engineering candidates we offer a Graduate Diploma in Civil Engineering, recognised by our accrediting body (the Joint Board of Moderators), which can be used as a pre-qualifying year for the Civil Engineering MSc.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>This MSc aims to equip students with the skills of analysis and design necessary for employment as professional civil engineers and give them a solid academic background for becoming chartered engineers. The Fluids route is for those students who want to further specialise in this subject, but also wish to improve their general background in other civil engineering disciplines.</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Offshore and Coastal Engineering
 Environmental Fluid Mechanics
@@ -766,235 +1031,236 @@
 Engineering Study of Rail Systems and Infrastructure</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/civil-engineering-fluids-msc</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>1 calendar year (full-time)</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>September 2023</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>£35,000</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>总分 6.5, 小分 6.0</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
         <is>
           <t>applicants with a good performance in the core subjects (design, structures, geotechnics, and fluids) or extensive work experience covering these areas may be considered.</t>
         </is>
       </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
         <is>
           <t>2:1</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr">
+      <c r="AG5" t="inlineStr">
         <is>
           <t>2:1</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>英国</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>University College London</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>伦敦大学学院</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>clinical ophthalmic practice msc</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>A minimum of a second-class Bachelor’s degree in a relevant discipline from a UK university or an overseas qualification of an equivalent standard. Candidates will need to have a professional healthcare qualification (in nursing or an allied healthcare profession). Students are also required to have at least one year’s ophthalmic experience and to be currently working in the field of ophthalmology.</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This programme will allow you to develop advanced knowledge of the eye, eye diseases and treatment and the research underpinning clinical practice. It is delivered by ophthalmologists, researchers and nurses who are at the forefront of ophthalmic research clinical practice at the Institute of Ophthalmology and Moorfields Eye Hospital Trust both institutions will be involved in the teaching.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Anatomy and Physiology
-Research and Statistics
-Ophthalmic Clinical Case Studies
-Clinical Care in Practice
-Physical assessment of the ophthalmic patient
-Ophthalmology Dissertation
-Glaucoma
-Medical Retina, Vitreoretinal, Systemic Diseases, Uveitis and Ocular Oncology
-Ophthalmic Accident and Emergency Clinical Practice
-Ophthalmic Theatre Practice</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/clinical-ophthalmic-practice-msc</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>2 calendar years (part-time)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>biochemical engineering msc</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Normal entry requirements are at least a second-class Bachelor's degree from a UK university or the equivalent from an approved overseas institution. Candidates offering recent industrial experience are also encouraged to apply. As with any engineering discipline numeracy skills are important for the quantitative description of biological and physical phenomena. Evidence of numerical ability is requested as either an A level in Mathematics (or in exceptional cases, in Physics) or some mathematics studied at university. The department provides mathematics tutoring for Master's students throughout the year adjusted to a candidate's ability.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Have you ever wondered how the latest life science discoveries, such as a novel stem cell therapy, can move from the lab into commercial scale production? Would you like to know whether it is possible to produce bio-polymers (plastics) and biofuels from municipal or agricultural waste? If you are thinking of a career in the pharma or biotech industries, the Biochemical Engineering MSc could be the right programme for you.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>未找到</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/biochemical-engineering-msc</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1 calendar year (full-time)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>September 2023</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>Fees to be confirmed</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>£35,000</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
         <is>
           <t>总分 6.5, 小分 6.0</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>candidates offering recent industrial experience are also encouraged to apply.</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
         <is>
           <t>2:2</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
+      <c r="AG6" t="inlineStr">
         <is>
           <t>2:2</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>英国</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>University College London</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>伦敦大学学院</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>manufacture and commercialisation of stem cell and gene therapies msc</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>A minimum of an upper second-class Bachelor's degree in relevant subject (e.g. Life Sciences, Biotechnology, Bioengineering, Environmental Science, Engineering, Chemistry or Business with a Biotechnology component) from a UK university or the equivalent from an approved overseas institution. Candidates offering recent industrial experience are also encouraged to apply.</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Rapid developments in the stem cell and gene therapy field have created skills shortages in this high-value manufacturing sector. This innovative and industrially-relevant MSc, which is co-developed and co-delivered by industry experts, provides key skills, practical training and expertise to develop future generations of engineers, scientists and business professionals with the breadth and depth required to manufacture and deliver 21st century medicines.</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Core Practical Research Skills
 MSc Advanced Therapy Research Project
@@ -1004,303 +1270,74 @@
 Commercialisation, Regulation and Ethics of Advanced Therapies</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/manufacture-and-commercialisation-stem-cell-and-gene-therapies-msc</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>1 calendar year (full-time)</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>September 2023</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>£41,500</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>总分 7.0, 小分 6.5</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>Level 2: Overall score of 7.0 and a minimum of 6.5 in each component</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>加分项</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
         <is>
           <t>candidates offering recent industrial experience are also encouraged to apply.</t>
         </is>
       </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>未要求</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
         <is>
           <t>2:1</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr">
+      <c r="AG7" t="inlineStr">
         <is>
           <t>2:1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>University College London</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>伦敦大学学院</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>biochemical engineering msc</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Normal entry requirements are at least a second-class Bachelor's degree from a UK university or the equivalent from an approved overseas institution. Candidates offering recent industrial experience are also encouraged to apply. As with any engineering discipline numeracy skills are important for the quantitative description of biological and physical phenomena. Evidence of numerical ability is requested as either an A level in Mathematics (or in exceptional cases, in Physics) or some mathematics studied at university. The department provides mathematics tutoring for Master's students throughout the year adjusted to a candidate's ability.</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Have you ever wondered how the latest life science discoveries, such as a novel stem cell therapy, can move from the lab into commercial scale production? Would you like to know whether it is possible to produce bio-polymers (plastics) and biofuels from municipal or agricultural waste? If you are thinking of a career in the pharma or biotech industries, the Biochemical Engineering MSc could be the right programme for you.</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>未找到</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/biochemical-engineering-msc</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>1 calendar year (full-time)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>September 2023</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>£35,000</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>总分 6.5, 小分 6.0</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>candidates offering recent industrial experience are also encouraged to apply.</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>2:2</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>2:2</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>英国</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>University College London</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>伦敦大学学院</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>global management of natural resources msc</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Normally a minimum of a second-class Bachelor’s degree in a relevant discipline – preferably engineering, Earth sciences, chemistry or finance/business - from a UK university or an overseas qualification of an equivalent standard. Relevant work experience may be taken into account.</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>More than ever, there is a growing demand for versatile specialists and managers in the globalised natural resources and commodities industries. These industries rely on effective collaboration between scientists, engineers, analysts, managers, and investors. This programme gives students the opportunity to develop an integrated understanding of resource genesis, production, supply, socio-environmental footprint and sustainable practice, which is now essential.</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Natural Gas Processing
-Minerals Usage, Extraction and Processing
-Prevention and Remediation of Environmental Contamination
-Dissertation
-Social Licensing
-Earth Resources and Sustainability
-Decision and Risk Analysis
-Business and Sustainability
-Renewable Energy in the Resources Sector
-Integrated Hydrogeology and Sustainable Water Management
-Geology for Global Managers and Engineers</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>https://www.ucl.ac.uk/prospective-students/graduate/taught-degrees/global-management-natural-resources-msc</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>1 calendar year (full-time)</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>September 2023</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>£38,300</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>总分 6.5, 小分 6.0</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Level 1: Overall score of 6.5 and a minimum of 6.0 in each component</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>relevant work experience may be taken into account.</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>未要求</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>2:2</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>2:2</t>
         </is>
       </c>
     </row>

</xml_diff>